<commit_message>
Uploaded wrong file, fixing
</commit_message>
<xml_diff>
--- a/table_of_results.xlsx
+++ b/table_of_results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B663EE3D-EB30-E349-9E99-9DE3CA2300E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7129C01F-199B-9B45-A296-DC2348B3A59E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34080" yWindow="3900" windowWidth="32880" windowHeight="18540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="32880" windowHeight="18540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V100" sheetId="2" r:id="rId1"/>
@@ -1050,6 +1050,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,30 +1158,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1532,21 +1532,21 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="114" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="117"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:30" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
@@ -1588,27 +1588,27 @@
       <c r="M2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="101"/>
+      <c r="N2" s="109"/>
       <c r="O2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="77" t="s">
+      <c r="P2" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="106"/>
-      <c r="X2" s="106"/>
-      <c r="Y2" s="106"/>
-      <c r="Z2" s="106"/>
-      <c r="AA2" s="106"/>
-      <c r="AB2" s="106"/>
-      <c r="AC2" s="106"/>
-      <c r="AD2" s="106"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="114"/>
+      <c r="V2" s="114"/>
+      <c r="W2" s="114"/>
+      <c r="X2" s="114"/>
+      <c r="Y2" s="114"/>
+      <c r="Z2" s="114"/>
+      <c r="AA2" s="114"/>
+      <c r="AB2" s="114"/>
+      <c r="AC2" s="114"/>
+      <c r="AD2" s="114"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1650,158 +1650,158 @@
         <f>L3/J3</f>
         <v>5.0184476632959818</v>
       </c>
-      <c r="N3" s="102"/>
+      <c r="N3" s="110"/>
       <c r="O3" s="4">
         <f>L3/MIN($N$16,K3*$N$15)</f>
         <v>0.37624678663239081</v>
       </c>
-      <c r="P3" s="75">
+      <c r="P3" s="83">
         <f>O3*100</f>
         <v>37.624678663239081</v>
       </c>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="104"/>
-      <c r="S3" s="104"/>
-      <c r="T3" s="104"/>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="106"/>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="106"/>
-      <c r="AB3" s="106"/>
-      <c r="AC3" s="106"/>
-      <c r="AD3" s="106"/>
+      <c r="Q3" s="112"/>
+      <c r="R3" s="112"/>
+      <c r="S3" s="112"/>
+      <c r="T3" s="112"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="114"/>
+      <c r="W3" s="114"/>
+      <c r="X3" s="114"/>
+      <c r="Y3" s="114"/>
+      <c r="Z3" s="114"/>
+      <c r="AA3" s="114"/>
+      <c r="AB3" s="114"/>
+      <c r="AC3" s="114"/>
+      <c r="AD3" s="114"/>
     </row>
     <row r="4" spans="1:30" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="85">
+      <c r="B4" s="93">
         <v>11.8</v>
       </c>
-      <c r="C4" s="80">
+      <c r="C4" s="88">
         <v>10.7</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="93">
+      <c r="E4" s="101">
         <v>11.8</v>
       </c>
-      <c r="F4" s="93">
+      <c r="F4" s="101">
         <v>10.7</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="94">
+      <c r="G4" s="93"/>
+      <c r="H4" s="102">
         <f>9897360000*1874</f>
         <v>18547652640000</v>
       </c>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94">
+      <c r="I4" s="102"/>
+      <c r="J4" s="102">
         <f>194.08+193.38</f>
         <v>387.46000000000004</v>
       </c>
-      <c r="K4" s="95">
+      <c r="K4" s="103">
         <f t="shared" ref="K4:K13" si="0">L4/J4</f>
         <v>4.4738178918438845</v>
       </c>
-      <c r="L4" s="80">
+      <c r="L4" s="88">
         <f>H4/F4/10^9</f>
         <v>1733.4254803738318</v>
       </c>
-      <c r="M4" s="96">
+      <c r="M4" s="104">
         <f t="shared" ref="M4:M13" si="1">L4/J4</f>
         <v>4.4738178918438845</v>
       </c>
-      <c r="N4" s="102"/>
-      <c r="O4" s="80">
+      <c r="N4" s="110"/>
+      <c r="O4" s="88">
         <f>L4/MIN($N$16,K4*$N$15)</f>
         <v>0.4980205655526993</v>
       </c>
-      <c r="P4" s="107">
+      <c r="P4" s="115">
         <f t="shared" ref="P4:P13" si="2">O4*100</f>
         <v>49.802056555269928</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="106"/>
-      <c r="X4" s="106"/>
-      <c r="Y4" s="106"/>
-      <c r="Z4" s="106"/>
-      <c r="AA4" s="106"/>
-      <c r="AB4" s="106"/>
-      <c r="AC4" s="106"/>
-      <c r="AD4" s="106"/>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="114"/>
+      <c r="Y4" s="114"/>
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="114"/>
     </row>
     <row r="5" spans="1:30" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="85">
+      <c r="B5" s="93">
         <v>203.23</v>
       </c>
-      <c r="C5" s="80">
+      <c r="C5" s="88">
         <v>191.84</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="94">
+      <c r="E5" s="102">
         <v>2.0322999999999999E-4</v>
       </c>
-      <c r="F5" s="94">
+      <c r="F5" s="102">
         <v>1.9260999999999999E-4</v>
       </c>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98">
+      <c r="G5" s="106"/>
+      <c r="H5" s="106">
         <v>75497584</v>
       </c>
-      <c r="I5" s="98"/>
-      <c r="J5" s="94">
+      <c r="I5" s="106"/>
+      <c r="J5" s="102">
         <f>359.77+353.42</f>
         <v>713.19</v>
       </c>
-      <c r="K5" s="95">
+      <c r="K5" s="103">
         <f t="shared" si="0"/>
         <v>0.54960285195032399</v>
       </c>
-      <c r="L5" s="80">
+      <c r="L5" s="88">
         <f>H5/F5/10^9</f>
         <v>391.97125798245162</v>
       </c>
-      <c r="M5" s="96">
+      <c r="M5" s="104">
         <f t="shared" si="1"/>
         <v>0.54960285195032399</v>
       </c>
-      <c r="N5" s="102"/>
-      <c r="O5" s="80">
+      <c r="N5" s="110"/>
+      <c r="O5" s="88">
         <f>L5/MIN(N17,K5*$N$15)</f>
         <v>0.91669665809768652</v>
       </c>
-      <c r="P5" s="107">
+      <c r="P5" s="115">
         <f t="shared" si="2"/>
         <v>91.669665809768645</v>
       </c>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="106"/>
-      <c r="AA5" s="106"/>
-      <c r="AB5" s="106"/>
-      <c r="AC5" s="106"/>
-      <c r="AD5" s="106"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="112"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="114"/>
+      <c r="V5" s="114"/>
+      <c r="W5" s="114"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="114"/>
+      <c r="Z5" s="114"/>
+      <c r="AA5" s="114"/>
+      <c r="AB5" s="114"/>
+      <c r="AC5" s="114"/>
+      <c r="AD5" s="114"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1839,29 +1839,29 @@
         <f t="shared" si="1"/>
         <v>0.22560685799913865</v>
       </c>
-      <c r="N6" s="102"/>
+      <c r="N6" s="110"/>
       <c r="O6" s="2">
         <f t="shared" ref="O6:O13" si="3">L6/MIN($N$16,K6*$N$15)</f>
         <v>0.64690231362467865</v>
       </c>
-      <c r="P6" s="75">
+      <c r="P6" s="83">
         <f t="shared" si="2"/>
         <v>64.69023136246787</v>
       </c>
-      <c r="Q6" s="104"/>
-      <c r="R6" s="104"/>
-      <c r="S6" s="104"/>
-      <c r="T6" s="104"/>
-      <c r="U6" s="106"/>
-      <c r="V6" s="106"/>
-      <c r="W6" s="106"/>
-      <c r="X6" s="106"/>
-      <c r="Y6" s="106"/>
-      <c r="Z6" s="106"/>
-      <c r="AA6" s="106"/>
-      <c r="AB6" s="106"/>
-      <c r="AC6" s="106"/>
-      <c r="AD6" s="106"/>
+      <c r="Q6" s="112"/>
+      <c r="R6" s="112"/>
+      <c r="S6" s="112"/>
+      <c r="T6" s="112"/>
+      <c r="U6" s="114"/>
+      <c r="V6" s="114"/>
+      <c r="W6" s="114"/>
+      <c r="X6" s="114"/>
+      <c r="Y6" s="114"/>
+      <c r="Z6" s="114"/>
+      <c r="AA6" s="114"/>
+      <c r="AB6" s="114"/>
+      <c r="AC6" s="114"/>
+      <c r="AD6" s="114"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1904,95 +1904,95 @@
         <f t="shared" si="1"/>
         <v>1.0893389656695045</v>
       </c>
-      <c r="N7" s="102"/>
+      <c r="N7" s="110"/>
       <c r="O7" s="2">
         <f t="shared" si="3"/>
         <v>0.72580077120822617</v>
       </c>
-      <c r="P7" s="75">
+      <c r="P7" s="83">
         <f t="shared" si="2"/>
         <v>72.580077120822622</v>
       </c>
-      <c r="Q7" s="104"/>
-      <c r="R7" s="104"/>
-      <c r="S7" s="104"/>
-      <c r="T7" s="104"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="106"/>
-      <c r="AA7" s="106"/>
-      <c r="AB7" s="106"/>
-      <c r="AC7" s="106"/>
-      <c r="AD7" s="106"/>
+      <c r="Q7" s="112"/>
+      <c r="R7" s="112"/>
+      <c r="S7" s="112"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="114"/>
+      <c r="V7" s="114"/>
+      <c r="W7" s="114"/>
+      <c r="X7" s="114"/>
+      <c r="Y7" s="114"/>
+      <c r="Z7" s="114"/>
+      <c r="AA7" s="114"/>
+      <c r="AB7" s="114"/>
+      <c r="AC7" s="114"/>
+      <c r="AD7" s="114"/>
     </row>
     <row r="8" spans="1:30" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="85">
+      <c r="B8" s="93">
         <v>5.6155220430000004</v>
       </c>
-      <c r="C8" s="80">
+      <c r="C8" s="88">
         <v>5.8482909999999997</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="94">
+      <c r="E8" s="102">
         <f>173017280/10^9</f>
         <v>0.17301728</v>
       </c>
-      <c r="F8" s="99">
+      <c r="F8" s="107">
         <v>0.1539229</v>
       </c>
-      <c r="G8" s="85"/>
-      <c r="H8" s="94">
+      <c r="G8" s="93"/>
+      <c r="H8" s="102">
         <f>50528256*1611</f>
         <v>81401020416</v>
       </c>
-      <c r="I8" s="94"/>
-      <c r="J8" s="82">
+      <c r="I8" s="102"/>
+      <c r="J8" s="90">
         <f>674.1+48.696</f>
         <v>722.79600000000005</v>
       </c>
-      <c r="K8" s="95">
+      <c r="K8" s="103">
         <f t="shared" si="0"/>
         <v>0.73166262605702104</v>
       </c>
-      <c r="L8" s="84">
+      <c r="L8" s="92">
         <f>H8/F8/10^9</f>
         <v>528.84281946351064</v>
       </c>
-      <c r="M8" s="96">
+      <c r="M8" s="104">
         <f t="shared" si="1"/>
         <v>0.73166262605702104</v>
       </c>
-      <c r="N8" s="102"/>
-      <c r="O8" s="80">
+      <c r="N8" s="110"/>
+      <c r="O8" s="88">
         <f t="shared" si="3"/>
         <v>0.92904370179948603</v>
       </c>
-      <c r="P8" s="107">
+      <c r="P8" s="115">
         <f t="shared" si="2"/>
         <v>92.9043701799486</v>
       </c>
-      <c r="Q8" s="104"/>
-      <c r="R8" s="104"/>
-      <c r="S8" s="104"/>
-      <c r="T8" s="104"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="106"/>
-      <c r="W8" s="106"/>
-      <c r="X8" s="106"/>
-      <c r="Y8" s="106"/>
-      <c r="Z8" s="106"/>
-      <c r="AA8" s="106"/>
-      <c r="AB8" s="106"/>
-      <c r="AC8" s="106"/>
-      <c r="AD8" s="106"/>
+      <c r="Q8" s="112"/>
+      <c r="R8" s="112"/>
+      <c r="S8" s="112"/>
+      <c r="T8" s="112"/>
+      <c r="U8" s="114"/>
+      <c r="V8" s="114"/>
+      <c r="W8" s="114"/>
+      <c r="X8" s="114"/>
+      <c r="Y8" s="114"/>
+      <c r="Z8" s="114"/>
+      <c r="AA8" s="114"/>
+      <c r="AB8" s="114"/>
+      <c r="AC8" s="114"/>
+      <c r="AD8" s="114"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -2035,160 +2035,160 @@
         <f t="shared" si="1"/>
         <v>98.03108823446361</v>
       </c>
-      <c r="N9" s="103"/>
+      <c r="N9" s="111"/>
       <c r="O9" s="2">
         <f t="shared" si="3"/>
         <v>0.18606954087489425</v>
       </c>
-      <c r="P9" s="75">
+      <c r="P9" s="83">
         <f t="shared" si="2"/>
         <v>18.606954087489424</v>
       </c>
-      <c r="Q9" s="104"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="T9" s="104"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="106"/>
-      <c r="AA9" s="106"/>
-      <c r="AB9" s="106"/>
-      <c r="AC9" s="106"/>
-      <c r="AD9" s="106"/>
+      <c r="Q9" s="112"/>
+      <c r="R9" s="112"/>
+      <c r="S9" s="112"/>
+      <c r="T9" s="112"/>
+      <c r="U9" s="114"/>
+      <c r="V9" s="114"/>
+      <c r="W9" s="114"/>
+      <c r="X9" s="114"/>
+      <c r="Y9" s="114"/>
+      <c r="Z9" s="114"/>
+      <c r="AA9" s="114"/>
+      <c r="AB9" s="114"/>
+      <c r="AC9" s="114"/>
+      <c r="AD9" s="114"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="85">
+      <c r="B10" s="93">
         <v>10.23</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="93">
         <v>7.8302800000000001</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="82">
+      <c r="E10" s="90">
         <f>0.008*1001</f>
         <v>8.0080000000000009</v>
       </c>
-      <c r="F10" s="99">
+      <c r="F10" s="107">
         <v>7.8070000000000004</v>
       </c>
-      <c r="G10" s="85"/>
-      <c r="H10" s="94">
+      <c r="G10" s="93"/>
+      <c r="H10" s="102">
         <f>6291454488*1001</f>
         <v>6297745942488</v>
       </c>
-      <c r="I10" s="94"/>
-      <c r="J10" s="82">
+      <c r="I10" s="102"/>
+      <c r="J10" s="90">
         <f>276.19</f>
         <v>276.19</v>
       </c>
-      <c r="K10" s="95">
+      <c r="K10" s="103">
         <f t="shared" si="0"/>
         <v>2.9207407325538304</v>
       </c>
-      <c r="L10" s="84">
+      <c r="L10" s="92">
         <f>H10/F10/10^9</f>
         <v>806.67938292404244</v>
       </c>
-      <c r="M10" s="96">
+      <c r="M10" s="104">
         <f t="shared" si="1"/>
         <v>2.9207407325538304</v>
       </c>
-      <c r="N10" s="103"/>
-      <c r="O10" s="80">
+      <c r="N10" s="111"/>
+      <c r="O10" s="88">
         <f t="shared" si="3"/>
         <v>0.35500000000000004</v>
       </c>
-      <c r="P10" s="107">
+      <c r="P10" s="115">
         <f t="shared" si="2"/>
         <v>35.500000000000007</v>
       </c>
-      <c r="Q10" s="104"/>
-      <c r="R10" s="104"/>
-      <c r="S10" s="104"/>
-      <c r="T10" s="104"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="106"/>
-      <c r="X10" s="106"/>
-      <c r="Y10" s="106"/>
-      <c r="Z10" s="106"/>
-      <c r="AA10" s="106"/>
-      <c r="AB10" s="106"/>
-      <c r="AC10" s="106"/>
-      <c r="AD10" s="106"/>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="112"/>
+      <c r="S10" s="112"/>
+      <c r="T10" s="112"/>
+      <c r="U10" s="114"/>
+      <c r="V10" s="114"/>
+      <c r="W10" s="114"/>
+      <c r="X10" s="114"/>
+      <c r="Y10" s="114"/>
+      <c r="Z10" s="114"/>
+      <c r="AA10" s="114"/>
+      <c r="AB10" s="114"/>
+      <c r="AC10" s="114"/>
+      <c r="AD10" s="114"/>
     </row>
     <row r="11" spans="1:30" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="85">
+      <c r="B11" s="93">
         <v>4.190816E-3</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="93">
         <v>4.0936000000000002E-3</v>
       </c>
-      <c r="D11" s="94" t="s">
+      <c r="D11" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="82">
+      <c r="E11" s="90">
         <v>4.190816E-3</v>
       </c>
-      <c r="F11" s="99">
+      <c r="F11" s="107">
         <v>4.0936000000000002E-3</v>
       </c>
-      <c r="G11" s="85"/>
-      <c r="H11" s="94">
+      <c r="G11" s="93"/>
+      <c r="H11" s="102">
         <f>35651584*100</f>
         <v>3565158400</v>
       </c>
-      <c r="I11" s="94"/>
-      <c r="J11" s="82">
+      <c r="I11" s="102"/>
+      <c r="J11" s="90">
         <f>198.37+364.96</f>
         <v>563.32999999999993</v>
       </c>
-      <c r="K11" s="95">
+      <c r="K11" s="103">
         <f t="shared" si="0"/>
         <v>1.5460037615666171</v>
       </c>
-      <c r="L11" s="84">
+      <c r="L11" s="92">
         <f>H11/F11/10^9</f>
         <v>870.91029900332228</v>
       </c>
-      <c r="M11" s="96">
+      <c r="M11" s="104">
         <f t="shared" si="1"/>
         <v>1.5460037615666171</v>
       </c>
-      <c r="N11" s="103"/>
-      <c r="O11" s="80">
+      <c r="N11" s="111"/>
+      <c r="O11" s="88">
         <f t="shared" si="3"/>
         <v>0.7240745501285345</v>
       </c>
-      <c r="P11" s="107">
+      <c r="P11" s="115">
         <f t="shared" si="2"/>
         <v>72.407455012853447</v>
       </c>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="104"/>
-      <c r="T11" s="104"/>
-      <c r="U11" s="106"/>
-      <c r="V11" s="106"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="106"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="106"/>
-      <c r="AA11" s="106"/>
-      <c r="AB11" s="106"/>
-      <c r="AC11" s="106"/>
-      <c r="AD11" s="106"/>
+      <c r="Q11" s="112"/>
+      <c r="R11" s="112"/>
+      <c r="S11" s="112"/>
+      <c r="T11" s="112"/>
+      <c r="U11" s="114"/>
+      <c r="V11" s="114"/>
+      <c r="W11" s="114"/>
+      <c r="X11" s="114"/>
+      <c r="Y11" s="114"/>
+      <c r="Z11" s="114"/>
+      <c r="AA11" s="114"/>
+      <c r="AB11" s="114"/>
+      <c r="AC11" s="114"/>
+      <c r="AD11" s="114"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -2230,29 +2230,29 @@
         <f t="shared" si="1"/>
         <v>0.10438777936706597</v>
       </c>
-      <c r="N12" s="103"/>
+      <c r="N12" s="111"/>
       <c r="O12" s="2">
         <f t="shared" si="3"/>
         <v>9.665809768637533E-2</v>
       </c>
-      <c r="P12" s="75">
+      <c r="P12" s="83">
         <f t="shared" si="2"/>
         <v>9.6658097686375335</v>
       </c>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="104"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="106"/>
-      <c r="AD12" s="106"/>
+      <c r="Q12" s="112"/>
+      <c r="R12" s="112"/>
+      <c r="S12" s="112"/>
+      <c r="T12" s="112"/>
+      <c r="U12" s="114"/>
+      <c r="V12" s="114"/>
+      <c r="W12" s="114"/>
+      <c r="X12" s="114"/>
+      <c r="Y12" s="114"/>
+      <c r="Z12" s="114"/>
+      <c r="AA12" s="114"/>
+      <c r="AB12" s="114"/>
+      <c r="AC12" s="114"/>
+      <c r="AD12" s="114"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -2264,7 +2264,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="24"/>
-      <c r="F13" s="88">
+      <c r="F13" s="96">
         <v>0.23799999999999999</v>
       </c>
       <c r="G13" s="52"/>
@@ -2288,80 +2288,80 @@
         <f t="shared" si="1"/>
         <v>0.20827406920480956</v>
       </c>
-      <c r="N13" s="103"/>
+      <c r="N13" s="111"/>
       <c r="O13" s="2">
         <f t="shared" si="3"/>
         <v>9.665809768637533E-2</v>
       </c>
-      <c r="P13" s="75">
+      <c r="P13" s="83">
         <f t="shared" si="2"/>
         <v>9.6658097686375335</v>
       </c>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="106"/>
-      <c r="W13" s="106"/>
-      <c r="X13" s="106"/>
-      <c r="Y13" s="106"/>
-      <c r="Z13" s="106"/>
-      <c r="AA13" s="106"/>
-      <c r="AB13" s="106"/>
-      <c r="AC13" s="106"/>
-      <c r="AD13" s="106"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="112"/>
+      <c r="S13" s="112"/>
+      <c r="T13" s="112"/>
+      <c r="U13" s="114"/>
+      <c r="V13" s="114"/>
+      <c r="W13" s="114"/>
+      <c r="X13" s="114"/>
+      <c r="Y13" s="114"/>
+      <c r="Z13" s="114"/>
+      <c r="AA13" s="114"/>
+      <c r="AB13" s="114"/>
+      <c r="AC13" s="114"/>
+      <c r="AD13" s="114"/>
     </row>
     <row r="14" spans="1:30" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="37"/>
       <c r="C14" s="8"/>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="110" t="s">
+      <c r="F14" s="97"/>
+      <c r="G14" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="75">
+      <c r="I14" s="83">
         <f>H3/10^9</f>
         <v>631.66999999999996</v>
       </c>
-      <c r="J14" s="75" t="s">
+      <c r="J14" s="83" t="s">
         <v>40</v>
       </c>
       <c r="M14" s="8"/>
-      <c r="N14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
-      <c r="U14" s="106"/>
-      <c r="V14" s="106"/>
-      <c r="W14" s="106"/>
-      <c r="X14" s="106"/>
-      <c r="Y14" s="106"/>
-      <c r="Z14" s="106"/>
-      <c r="AA14" s="106"/>
-      <c r="AB14" s="106"/>
-      <c r="AC14" s="106"/>
-      <c r="AD14" s="106"/>
+      <c r="N14" s="112"/>
+      <c r="Q14" s="112"/>
+      <c r="R14" s="112"/>
+      <c r="S14" s="112"/>
+      <c r="T14" s="112"/>
+      <c r="U14" s="114"/>
+      <c r="V14" s="114"/>
+      <c r="W14" s="114"/>
+      <c r="X14" s="114"/>
+      <c r="Y14" s="114"/>
+      <c r="Z14" s="114"/>
+      <c r="AA14" s="114"/>
+      <c r="AB14" s="114"/>
+      <c r="AC14" s="114"/>
+      <c r="AD14" s="114"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B15" s="8"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="89" t="s">
+      <c r="F15" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="89">
+      <c r="G15" s="97">
         <f>ABS(E3-F3)/AVERAGE(E3,F3)*100</f>
         <v>38.353586459299045</v>
       </c>
-      <c r="I15" s="75">
+      <c r="I15" s="83">
         <f>H4/10^9</f>
         <v>18547.65264</v>
       </c>
-      <c r="J15" s="75">
+      <c r="J15" s="83">
         <f>J3*F3</f>
         <v>125.86960000000001</v>
       </c>
@@ -2371,45 +2371,45 @@
       <c r="N15" s="2">
         <v>778</v>
       </c>
-      <c r="O15" s="75" t="s">
+      <c r="O15" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="P15" s="100">
+      <c r="P15" s="108">
         <f>N16/N15</f>
         <v>19.280205655526991</v>
       </c>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
-      <c r="U15" s="106"/>
-      <c r="V15" s="106"/>
-      <c r="W15" s="106"/>
-      <c r="X15" s="106"/>
-      <c r="Y15" s="106"/>
-      <c r="Z15" s="106"/>
-      <c r="AA15" s="106"/>
-      <c r="AB15" s="106"/>
-      <c r="AC15" s="106"/>
-      <c r="AD15" s="106"/>
+      <c r="Q15" s="112"/>
+      <c r="R15" s="112"/>
+      <c r="S15" s="112"/>
+      <c r="T15" s="112"/>
+      <c r="U15" s="114"/>
+      <c r="V15" s="114"/>
+      <c r="W15" s="114"/>
+      <c r="X15" s="114"/>
+      <c r="Y15" s="114"/>
+      <c r="Z15" s="114"/>
+      <c r="AA15" s="114"/>
+      <c r="AB15" s="114"/>
+      <c r="AC15" s="114"/>
+      <c r="AD15" s="114"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="89" t="s">
+      <c r="F16" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="89">
+      <c r="G16" s="97">
         <f t="shared" ref="G16:G23" si="4">ABS(E4-F4)/AVERAGE(E4,F4)*100</f>
         <v>9.777777777777791</v>
       </c>
-      <c r="I16" s="75">
+      <c r="I16" s="83">
         <f t="shared" ref="I16:I24" si="5">H5/10^9</f>
         <v>7.5497584000000006E-2</v>
       </c>
-      <c r="J16" s="109">
+      <c r="J16" s="117">
         <f t="shared" ref="J16:J24" si="6">J4*F4</f>
         <v>4145.8220000000001</v>
       </c>
@@ -2419,38 +2419,38 @@
       <c r="N16" s="1">
         <v>15000</v>
       </c>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
-      <c r="U16" s="106"/>
-      <c r="V16" s="106"/>
-      <c r="W16" s="106"/>
-      <c r="X16" s="106"/>
-      <c r="Y16" s="106"/>
-      <c r="Z16" s="106"/>
-      <c r="AA16" s="106"/>
-      <c r="AB16" s="106"/>
-      <c r="AC16" s="106"/>
-      <c r="AD16" s="106"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="112"/>
+      <c r="T16" s="112"/>
+      <c r="U16" s="114"/>
+      <c r="V16" s="114"/>
+      <c r="W16" s="114"/>
+      <c r="X16" s="114"/>
+      <c r="Y16" s="114"/>
+      <c r="Z16" s="114"/>
+      <c r="AA16" s="114"/>
+      <c r="AB16" s="114"/>
+      <c r="AC16" s="114"/>
+      <c r="AD16" s="114"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="89" t="s">
+      <c r="F17" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="89">
+      <c r="G17" s="97">
         <f>ABS(E5-F5)/AVERAGE(E5,F5)*100</f>
         <v>5.3658043654001641</v>
       </c>
-      <c r="I17" s="75">
+      <c r="I17" s="83">
         <f t="shared" si="5"/>
         <v>1.6252928E-2</v>
       </c>
-      <c r="J17" s="109">
+      <c r="J17" s="117">
         <f t="shared" si="6"/>
         <v>0.13736752590000001</v>
       </c>
@@ -2461,108 +2461,108 @@
         <f>7660</f>
         <v>7660</v>
       </c>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="104"/>
-      <c r="U17" s="106"/>
-      <c r="V17" s="106"/>
-      <c r="W17" s="106"/>
-      <c r="X17" s="106"/>
-      <c r="Y17" s="106"/>
-      <c r="Z17" s="106"/>
-      <c r="AA17" s="106"/>
-      <c r="AB17" s="106"/>
-      <c r="AC17" s="106"/>
-      <c r="AD17" s="106"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="112"/>
+      <c r="T17" s="112"/>
+      <c r="U17" s="114"/>
+      <c r="V17" s="114"/>
+      <c r="W17" s="114"/>
+      <c r="X17" s="114"/>
+      <c r="Y17" s="114"/>
+      <c r="Z17" s="114"/>
+      <c r="AA17" s="114"/>
+      <c r="AB17" s="114"/>
+      <c r="AC17" s="114"/>
+      <c r="AD17" s="114"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="89" t="s">
+      <c r="F18" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="89">
+      <c r="G18" s="97">
         <f t="shared" si="4"/>
         <v>20.789383079282619</v>
       </c>
-      <c r="I18" s="75">
+      <c r="I18" s="83">
         <f t="shared" si="5"/>
         <v>0.50390040000000003</v>
       </c>
-      <c r="J18" s="75">
+      <c r="J18" s="83">
         <f t="shared" si="6"/>
         <v>7.2040930599999983E-2</v>
       </c>
-      <c r="Q18" s="104"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
-      <c r="T18" s="104"/>
-      <c r="U18" s="106"/>
-      <c r="V18" s="106"/>
-      <c r="W18" s="106"/>
-      <c r="X18" s="106"/>
-      <c r="Y18" s="106"/>
-      <c r="Z18" s="106"/>
-      <c r="AA18" s="106"/>
-      <c r="AB18" s="106"/>
-      <c r="AC18" s="106"/>
-      <c r="AD18" s="106"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="112"/>
+      <c r="S18" s="112"/>
+      <c r="T18" s="112"/>
+      <c r="U18" s="114"/>
+      <c r="V18" s="114"/>
+      <c r="W18" s="114"/>
+      <c r="X18" s="114"/>
+      <c r="Y18" s="114"/>
+      <c r="Z18" s="114"/>
+      <c r="AA18" s="114"/>
+      <c r="AB18" s="114"/>
+      <c r="AC18" s="114"/>
+      <c r="AD18" s="114"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="89" t="s">
+      <c r="F19" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="89">
+      <c r="G19" s="97">
         <f t="shared" si="4"/>
         <v>179.6084307920934</v>
       </c>
-      <c r="I19" s="75">
+      <c r="I19" s="83">
         <f t="shared" si="5"/>
         <v>81.401020415999994</v>
       </c>
-      <c r="J19" s="75">
+      <c r="J19" s="83">
         <f>J7*F7</f>
         <v>0.46257447487000003</v>
       </c>
-      <c r="Q19" s="106"/>
-      <c r="R19" s="106"/>
-      <c r="S19" s="106"/>
-      <c r="T19" s="106"/>
-      <c r="U19" s="106"/>
-      <c r="V19" s="106"/>
-      <c r="W19" s="106"/>
-      <c r="X19" s="106"/>
-      <c r="Y19" s="106"/>
-      <c r="Z19" s="106"/>
-      <c r="AA19" s="106"/>
-      <c r="AB19" s="106"/>
-      <c r="AC19" s="106"/>
-      <c r="AD19" s="106"/>
+      <c r="Q19" s="114"/>
+      <c r="R19" s="114"/>
+      <c r="S19" s="114"/>
+      <c r="T19" s="114"/>
+      <c r="U19" s="114"/>
+      <c r="V19" s="114"/>
+      <c r="W19" s="114"/>
+      <c r="X19" s="114"/>
+      <c r="Y19" s="114"/>
+      <c r="Z19" s="114"/>
+      <c r="AA19" s="114"/>
+      <c r="AB19" s="114"/>
+      <c r="AC19" s="114"/>
+      <c r="AD19" s="114"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="89" t="s">
+      <c r="F20" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="89">
+      <c r="G20" s="97">
         <f t="shared" si="4"/>
         <v>11.680656687715771</v>
       </c>
-      <c r="I20" s="75">
+      <c r="I20" s="83">
         <f>I9/10^9</f>
         <v>20.342517730000001</v>
       </c>
-      <c r="J20" s="109">
+      <c r="J20" s="117">
         <f t="shared" si="6"/>
         <v>111.2548564284</v>
       </c>
@@ -2572,18 +2572,18 @@
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="89" t="s">
+      <c r="F21" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="89">
+      <c r="G21" s="97">
         <f t="shared" si="4"/>
         <v>188.21053142382277</v>
       </c>
-      <c r="I21" s="75">
+      <c r="I21" s="83">
         <f t="shared" si="5"/>
         <v>6297.7459424879999</v>
       </c>
-      <c r="J21" s="75">
+      <c r="J21" s="83">
         <f t="shared" si="6"/>
         <v>0.20751088349999999</v>
       </c>
@@ -2593,18 +2593,18 @@
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="89" t="s">
+      <c r="F22" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="89">
+      <c r="G22" s="97">
         <f t="shared" si="4"/>
         <v>2.5418906101802148</v>
       </c>
-      <c r="I22" s="75">
+      <c r="I22" s="83">
         <f t="shared" si="5"/>
         <v>3.5651584000000001</v>
       </c>
-      <c r="J22" s="109">
+      <c r="J22" s="117">
         <f t="shared" si="6"/>
         <v>2156.21533</v>
       </c>
@@ -2615,18 +2615,18 @@
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="89" t="s">
+      <c r="F23" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="89">
+      <c r="G23" s="97">
         <f t="shared" si="4"/>
         <v>2.3469608479342372</v>
       </c>
-      <c r="I23" s="75">
+      <c r="I23" s="83">
         <f t="shared" si="5"/>
         <v>1.8682907200000001</v>
       </c>
-      <c r="J23" s="109">
+      <c r="J23" s="117">
         <f t="shared" si="6"/>
         <v>2.3060476879999996</v>
       </c>
@@ -2637,18 +2637,18 @@
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="89" t="s">
+      <c r="F24" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="89">
+      <c r="G24" s="97">
         <f>ABS(E12-F12)/AVERAGE(E12,F12)*100</f>
         <v>47.435897435897445</v>
       </c>
-      <c r="I24" s="75">
+      <c r="I24" s="83">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J24" s="111">
+      <c r="J24" s="119">
         <f t="shared" si="6"/>
         <v>17.897600000000001</v>
       </c>
@@ -2660,7 +2660,7 @@
       <c r="D25" s="33"/>
       <c r="E25" s="8"/>
       <c r="F25" s="33"/>
-      <c r="G25" s="91"/>
+      <c r="G25" s="99"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
@@ -2694,102 +2694,102 @@
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="86"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="90"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="98"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="86"/>
+      <c r="G29" s="94"/>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="86"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="86"/>
+      <c r="A30" s="94"/>
+      <c r="B30" s="95"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="94"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="86"/>
+      <c r="G30" s="94"/>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="86"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="86"/>
+      <c r="A31" s="94"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="94"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="86"/>
+      <c r="G31" s="94"/>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A32" s="86"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="86"/>
+      <c r="A32" s="94"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="94"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="86"/>
+      <c r="G32" s="94"/>
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="86"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="86"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="94"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="86"/>
+      <c r="G33" s="94"/>
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="86"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="86"/>
+      <c r="A34" s="94"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="94"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="86"/>
+      <c r="G34" s="94"/>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="86"/>
-      <c r="B35" s="87"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="86"/>
+      <c r="A35" s="94"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="94"/>
       <c r="E35" s="8"/>
       <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="86"/>
-      <c r="B36" s="87"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="86"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="94"/>
       <c r="E36" s="8"/>
       <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="86"/>
-      <c r="B37" s="87"/>
-      <c r="C37" s="87"/>
-      <c r="D37" s="86"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="94"/>
       <c r="E37" s="8"/>
       <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="86"/>
-      <c r="B38" s="87"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="86"/>
+      <c r="A38" s="94"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="94"/>
       <c r="E38" s="8"/>
       <c r="G38" s="26"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="86"/>
-      <c r="B39" s="87"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="86"/>
+      <c r="A39" s="94"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="94"/>
       <c r="E39" s="8"/>
       <c r="G39" s="26"/>
     </row>
@@ -2822,8 +2822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2840,12 +2840,12 @@
       <c r="A1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="119"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -2869,10 +2869,10 @@
       <c r="H2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="75" t="s">
+      <c r="I2" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="78"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
@@ -2883,72 +2883,95 @@
       <c r="B3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="17" t="e">
-        <f t="shared" ref="D3:D13" si="0">E3/C3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="1"/>
-      <c r="H3" s="2" t="e">
-        <f t="shared" ref="H3:H13" si="1">E3/MIN($I$19,$I$18*D3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I3" s="75" t="e">
+      <c r="C3" s="23">
+        <f>27.971+8.613</f>
+        <v>36.584000000000003</v>
+      </c>
+      <c r="D3" s="17">
+        <f t="shared" ref="D3:D14" si="0">E3/C3</f>
+        <v>5.9156735184780231</v>
+      </c>
+      <c r="E3" s="57">
+        <v>216.41900000000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.8959999999999999</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H14" si="1">E3/MIN($I$19,$I$18*D3)</f>
+        <v>0.54602985074626875</v>
+      </c>
+      <c r="I3" s="83">
         <f>H3*100</f>
-        <v>#DIV/0!</v>
+        <v>54.602985074626872</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83" t="e">
+      <c r="C4" s="90">
+        <f>(21.701 +10.878)*197.778/F4</f>
+        <v>32.638329319955311</v>
+      </c>
+      <c r="D4" s="91">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
-      <c r="H4" s="2" t="e">
+        <v>2.870172237860491</v>
+      </c>
+      <c r="E4" s="92">
+        <f>92.277*200.415/F4</f>
+        <v>93.67762670428381</v>
+      </c>
+      <c r="F4" s="93">
+        <v>197.41848300000001</v>
+      </c>
+      <c r="H4" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" s="75" t="e">
+        <v>0.48713924358142258</v>
+      </c>
+      <c r="I4" s="83">
         <f t="shared" ref="I4:I13" si="2">H4*100</f>
-        <v>#DIV/0!</v>
+        <v>48.713924358142258</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="83" t="e">
+      <c r="C5" s="90">
+        <f>10.637+9.809</f>
+        <v>20.445999999999998</v>
+      </c>
+      <c r="D5" s="91">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="85"/>
-      <c r="H5" s="2" t="e">
+        <v>0.48425119827839191</v>
+      </c>
+      <c r="E5" s="92">
+        <v>9.9009999999999998</v>
+      </c>
+      <c r="F5" s="93">
+        <f>6.97/1000</f>
+        <v>6.9699999999999996E-3</v>
+      </c>
+      <c r="H5" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I5" s="75" t="e">
+        <v>0.30516417910447763</v>
+      </c>
+      <c r="I5" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>30.516417910447764</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -2961,20 +2984,28 @@
       <c r="B6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="18" t="e">
+      <c r="C6" s="5">
+        <f>5.672+4.953</f>
+        <v>10.625</v>
+      </c>
+      <c r="D6" s="18">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="1"/>
-      <c r="H6" s="2" t="e">
+        <v>0.26287058823529413</v>
+      </c>
+      <c r="E6" s="42">
+        <v>2.7930000000000001</v>
+      </c>
+      <c r="F6" s="1">
+        <f>6.89/1000</f>
+        <v>6.8899999999999994E-3</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" s="75" t="e">
+        <v>0.15858208955223879</v>
+      </c>
+      <c r="I6" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>15.85820895522388</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -2987,46 +3018,60 @@
       <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="18" t="e">
+      <c r="C7" s="5">
+        <f>20.705+0.13</f>
+        <v>20.834999999999997</v>
+      </c>
+      <c r="D7" s="18">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="1"/>
-      <c r="H7" s="2" t="e">
+        <v>2.0319174466042718</v>
+      </c>
+      <c r="E7" s="42">
+        <v>42.335000000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="H7" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" s="75" t="e">
+        <v>0.31097014925373134</v>
+      </c>
+      <c r="I7" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>31.097014925373134</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="83" t="e">
+      <c r="C8" s="90">
+        <f>13.674+0.255</f>
+        <v>13.929</v>
+      </c>
+      <c r="D8" s="91">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" s="84"/>
-      <c r="F8" s="85"/>
-      <c r="H8" s="32" t="e">
+        <v>1.481226218680451</v>
+      </c>
+      <c r="E8" s="92">
+        <v>20.632000000000001</v>
+      </c>
+      <c r="F8" s="93">
+        <v>8.4603599999999997</v>
+      </c>
+      <c r="H8" s="32">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" s="79" t="e">
+        <v>0.20789552238805969</v>
+      </c>
+      <c r="I8" s="87">
         <f>H8*100</f>
-        <v>#DIV/0!</v>
+        <v>20.789552238805971</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -3039,72 +3084,95 @@
       <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="18" t="e">
+      <c r="C9" s="5">
+        <f>1.905+0.064</f>
+        <v>1.9690000000000001</v>
+      </c>
+      <c r="D9" s="18">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="1"/>
-      <c r="H9" s="75" t="e">
+        <v>38.831894362620616</v>
+      </c>
+      <c r="E9" s="42">
+        <v>76.459999999999994</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3.13</v>
+      </c>
+      <c r="H9" s="83">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" s="75" t="e">
+        <v>6.4252100840336127E-2</v>
+      </c>
+      <c r="I9" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>6.4252100840336128</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="83" t="e">
+      <c r="C10" s="90">
+        <f>18.488+8.527</f>
+        <v>27.015000000000001</v>
+      </c>
+      <c r="D10" s="91">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="85"/>
-      <c r="H10" s="75" t="e">
+        <v>0.80103646122524519</v>
+      </c>
+      <c r="E10" s="92">
+        <v>21.64</v>
+      </c>
+      <c r="F10" s="93">
+        <v>222.27</v>
+      </c>
+      <c r="H10" s="83">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" s="75" t="e">
+        <v>0.40320895522388067</v>
+      </c>
+      <c r="I10" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>40.320895522388071</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="83" t="e">
+      <c r="C11" s="90">
+        <f>43.173+21.168</f>
+        <v>64.341000000000008</v>
+      </c>
+      <c r="D11" s="91">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="85"/>
-      <c r="H11" s="75" t="e">
+        <v>1.5364740320605912</v>
+      </c>
+      <c r="E11" s="92">
+        <f>37748736/381847</f>
+        <v>98.858275696810509</v>
+      </c>
+      <c r="F11" s="93">
+        <f>381847/10^9</f>
+        <v>3.8184699999999999E-4</v>
+      </c>
+      <c r="H11" s="83">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="75" t="e">
+        <v>0.96031343283582105</v>
+      </c>
+      <c r="I11" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>96.031343283582103</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -3117,20 +3185,27 @@
       <c r="B12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="19" t="e">
+      <c r="C12" s="24">
+        <f>5.468+3.205</f>
+        <v>8.673</v>
+      </c>
+      <c r="D12" s="19">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="1"/>
-      <c r="H12" s="75" t="e">
+        <v>5.9227487605211575</v>
+      </c>
+      <c r="E12" s="58">
+        <v>51.368000000000002</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3.556</v>
+      </c>
+      <c r="H12" s="83">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" s="75" t="e">
+        <v>0.12944776119402987</v>
+      </c>
+      <c r="I12" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>12.944776119402986</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -3143,20 +3218,25 @@
       <c r="B13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="20" t="e">
+      <c r="C13" s="25">
+        <f>5.468+3.205</f>
+        <v>8.673</v>
+      </c>
+      <c r="D13" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" s="59"/>
+        <v>33.350513086590574</v>
+      </c>
+      <c r="E13" s="59">
+        <v>289.24900000000002</v>
+      </c>
       <c r="F13" s="1"/>
-      <c r="H13" s="75" t="e">
+      <c r="H13" s="83">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" s="75" t="e">
+        <v>0.24306638655462187</v>
+      </c>
+      <c r="I13" s="83">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>24.306638655462187</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -3171,10 +3251,10 @@
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="83" t="s">
         <v>49</v>
       </c>
       <c r="H15" s="8"/>
@@ -3184,119 +3264,128 @@
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D16" s="75">
+      <c r="D16" s="83">
         <f>C3*F3</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="75">
+        <v>105.947264</v>
+      </c>
+      <c r="E16" s="83">
         <f>F3*E3</f>
-        <v>0</v>
+        <v>626.74942399999998</v>
       </c>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D17" s="109">
+      <c r="D17" s="117">
         <f t="shared" ref="D17:D25" si="3">C4*F4</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="75">
+        <v>6443.4094619999996</v>
+      </c>
+      <c r="E17" s="83">
         <f>F4*E4</f>
-        <v>0</v>
+        <v>18493.694954999999</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D18" s="109">
+      <c r="D18" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="75">
+        <v>0.14250861999999997</v>
+      </c>
+      <c r="E18" s="83">
         <f t="shared" ref="E18:E25" si="4">F5*E5</f>
-        <v>0</v>
+        <v>6.900996999999999E-2</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="K18" s="75" t="s">
+      <c r="I18" s="1">
+        <v>67</v>
+      </c>
+      <c r="K18" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="75" t="e">
+      <c r="L18" s="83">
         <f>I19/I18</f>
-        <v>#DIV/0!</v>
+        <v>17.761194029850746</v>
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D19" s="75">
+      <c r="D19" s="83">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="75">
+        <v>7.320625E-2</v>
+      </c>
+      <c r="E19" s="83">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.924377E-2</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <v>1190</v>
+      </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D20" s="75">
+      <c r="D20" s="83">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="75">
+        <v>10.750859999999999</v>
+      </c>
+      <c r="E20" s="83">
         <f>F7*E7</f>
-        <v>0</v>
+        <v>21.844860000000001</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <v>330</v>
+      </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D21" s="109">
+      <c r="D21" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="75">
+        <v>117.84435444</v>
+      </c>
+      <c r="E21" s="83">
         <f>F8*E8</f>
-        <v>0</v>
+        <v>174.55414752000001</v>
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D22" s="75">
+      <c r="D22" s="83">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="75">
+        <v>6.1629699999999996</v>
+      </c>
+      <c r="E22" s="83">
         <f>F9*E9</f>
-        <v>0</v>
+        <v>239.31979999999996</v>
       </c>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D23" s="109">
+      <c r="D23" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="75">
+        <v>6004.6240500000004</v>
+      </c>
+      <c r="E23" s="83">
         <f>F10*E10</f>
-        <v>0</v>
+        <v>4809.9228000000003</v>
       </c>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D24" s="109">
+      <c r="D24" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="75"/>
+        <v>2.4568417827000002E-2</v>
+      </c>
+      <c r="E24" s="83">
+        <f>3774873600/10^9</f>
+        <v>3.7748735999999998</v>
+      </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D25" s="75">
+      <c r="D25" s="83">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="75">
+        <v>30.841187999999999</v>
+      </c>
+      <c r="E25" s="83">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>182.66460800000002</v>
       </c>
     </row>
   </sheetData>
@@ -3330,15 +3419,15 @@
       <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="119"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3383,7 +3472,7 @@
       <c r="C3" s="49">
         <v>1.9159999999999999</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D3" s="82">
         <f>(27.971+8.613)*2896000000</f>
         <v>105947264000.00002</v>
       </c>
@@ -3834,39 +3923,39 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="85" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E15" s="77">
+      <c r="E15" s="85">
         <f>E3/10^9</f>
         <v>658.88131200500004</v>
       </c>
-      <c r="F15" s="77">
+      <c r="F15" s="85">
         <f>D3/10^9</f>
         <v>105.94726400000002</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E16" s="77">
+      <c r="E16" s="85">
         <f t="shared" ref="E16:E24" si="8">E4/10^9</f>
         <v>18547.652640003998</v>
       </c>
-      <c r="F16" s="108">
+      <c r="F16" s="116">
         <f t="shared" ref="F16:F25" si="9">D4/10^9</f>
         <v>5409.5271873920001</v>
       </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E17" s="77">
+      <c r="E17" s="85">
         <f>E5/10^9</f>
         <v>7.5497584000000006E-2</v>
       </c>
-      <c r="F17" s="108">
+      <c r="F17" s="116">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3885,11 +3974,11 @@
       </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E18" s="77">
+      <c r="E18" s="85">
         <f t="shared" si="8"/>
         <v>2.4641535999999999E-2</v>
       </c>
-      <c r="F18" s="77">
+      <c r="F18" s="85">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3901,11 +3990,11 @@
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E19" s="77">
+      <c r="E19" s="85">
         <f t="shared" si="8"/>
         <v>10.035029</v>
       </c>
-      <c r="F19" s="77">
+      <c r="F19" s="85">
         <f t="shared" si="9"/>
         <v>5.9751344</v>
       </c>
@@ -3917,61 +4006,61 @@
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E20" s="77">
+      <c r="E20" s="85">
         <f t="shared" si="8"/>
         <v>81.470365841000003</v>
       </c>
-      <c r="F20" s="108">
+      <c r="F20" s="116">
         <f t="shared" si="9"/>
         <v>42.050067712000001</v>
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E21" s="77">
+      <c r="E21" s="85">
         <f t="shared" si="8"/>
         <v>1.6280999999999999E-5</v>
       </c>
-      <c r="F21" s="77">
+      <c r="F21" s="85">
         <f t="shared" si="9"/>
         <v>2.6153490559999999</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E22" s="77">
+      <c r="E22" s="85">
         <f t="shared" si="8"/>
         <v>3148.873729506</v>
       </c>
-      <c r="F22" s="108">
+      <c r="F22" s="116">
         <f t="shared" si="9"/>
         <v>11411.040990848</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E23" s="77">
+      <c r="E23" s="85">
         <f t="shared" si="8"/>
         <v>3.5651584000000001</v>
       </c>
-      <c r="F23" s="108">
+      <c r="F23" s="116">
         <f t="shared" si="9"/>
         <v>0.98446239999999996</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E24" s="77">
+      <c r="E24" s="85">
         <f t="shared" si="8"/>
         <v>220.849212771</v>
       </c>
-      <c r="F24" s="77">
+      <c r="F24" s="85">
         <f t="shared" si="9"/>
         <v>7.1914740479999999</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E25" s="77">
+      <c r="E25" s="85">
         <f>E13/10^9</f>
         <v>0</v>
       </c>
-      <c r="F25" s="77">
+      <c r="F25" s="85">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4001,249 +4090,249 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="77" t="s">
+      <c r="F2" s="85" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="83">
         <f>'V100'!P3</f>
         <v>37.624678663239081</v>
       </c>
-      <c r="D3" s="75" t="e">
+      <c r="D3" s="83">
         <f>'Gen9'!I3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E3" s="75">
+        <v>54.602985074626872</v>
+      </c>
+      <c r="E3" s="83">
         <f>SKX!K3</f>
         <v>25.839283554133424</v>
       </c>
-      <c r="F3" s="75" t="e">
+      <c r="F3" s="83">
         <f>3/(1/C3+1/D3+1/E3)</f>
-        <v>#DIV/0!</v>
+        <v>35.888137865402534</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="75">
+      <c r="C4" s="83">
         <f>'V100'!P4</f>
         <v>49.802056555269928</v>
       </c>
-      <c r="D4" s="75" t="e">
+      <c r="D4" s="83">
         <f>'Gen9'!I4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="75">
+        <v>48.713924358142258</v>
+      </c>
+      <c r="E4" s="83">
         <f>SKX!K4</f>
         <v>35.89118902039673</v>
       </c>
-      <c r="F4" s="75" t="e">
+      <c r="F4" s="83">
         <f t="shared" ref="F4:F15" si="0">3/(1/C4+1/D4+1/E4)</f>
-        <v>#DIV/0!</v>
+        <v>43.815132568145579</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="75">
+      <c r="C5" s="83">
         <f>'V100'!P5</f>
         <v>91.669665809768645</v>
       </c>
-      <c r="D5" s="75" t="e">
+      <c r="D5" s="83">
         <f>'Gen9'!I5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" s="75" t="e">
+        <v>30.516417910447764</v>
+      </c>
+      <c r="E5" s="83" t="e">
         <f>SKX!K5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="75" t="e">
+      <c r="F5" s="83" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="75">
+      <c r="C6" s="83">
         <f>'V100'!P6</f>
         <v>64.69023136246787</v>
       </c>
-      <c r="D6" s="75" t="e">
+      <c r="D6" s="83">
         <f>'Gen9'!I6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="75" t="e">
+        <v>15.85820895522388</v>
+      </c>
+      <c r="E6" s="83" t="e">
         <f>SKX!K6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="75" t="e">
+      <c r="F6" s="83" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="83">
         <f>'V100'!P7</f>
         <v>72.580077120822622</v>
       </c>
-      <c r="D7" s="75" t="e">
+      <c r="D7" s="83">
         <f>'Gen9'!I7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="75">
+        <v>31.097014925373134</v>
+      </c>
+      <c r="E7" s="83">
         <f>SKX!K7</f>
         <v>82.121143485431546</v>
       </c>
-      <c r="F7" s="75" t="e">
+      <c r="F7" s="83">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>51.624054054667745</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="83">
         <f>'V100'!P8</f>
         <v>92.9043701799486</v>
       </c>
-      <c r="D8" s="75" t="e">
+      <c r="D8" s="83">
         <f>'Gen9'!I8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" s="75">
+        <v>20.789552238805971</v>
+      </c>
+      <c r="E8" s="83">
         <f>SKX!K8</f>
         <v>9.9794638656180137</v>
       </c>
-      <c r="F8" s="75" t="e">
+      <c r="F8" s="83">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>18.859547530583541</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="75">
+      <c r="C9" s="83">
         <f>'V100'!P9</f>
         <v>18.606954087489424</v>
       </c>
-      <c r="D9" s="75" t="e">
+      <c r="D9" s="83">
         <f>'Gen9'!I9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E9" s="75">
+        <v>6.4252100840336128</v>
+      </c>
+      <c r="E9" s="83">
         <f>SKX!K9</f>
         <v>0.73181181263640949</v>
       </c>
-      <c r="F9" s="75" t="e">
+      <c r="F9" s="83">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.9037323156565775</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="75">
+      <c r="C10" s="83">
         <f>'V100'!P10</f>
         <v>35.500000000000007</v>
       </c>
-      <c r="D10" s="75" t="e">
+      <c r="D10" s="83">
         <f>'Gen9'!I10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" s="75">
+        <v>40.320895522388071</v>
+      </c>
+      <c r="E10" s="83">
         <f>SKX!K10</f>
         <v>78.157447959792606</v>
       </c>
-      <c r="F10" s="75" t="e">
+      <c r="F10" s="83">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>45.617152300957841</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="75">
+      <c r="C11" s="83">
         <f>'V100'!P11</f>
         <v>72.407455012853447</v>
       </c>
-      <c r="D11" s="75" t="e">
+      <c r="D11" s="83">
         <f>'Gen9'!I11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="75">
+        <v>96.031343283582103</v>
+      </c>
+      <c r="E11" s="83">
         <f>SKX!K11</f>
         <v>16.478459679711456</v>
       </c>
-      <c r="F11" s="75" t="e">
+      <c r="F11" s="83">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>35.33182581495447</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="75">
+      <c r="C12" s="83">
         <f>'V100'!P12</f>
         <v>9.6658097686375335</v>
       </c>
-      <c r="D12" s="75" t="e">
+      <c r="D12" s="83">
         <f>'Gen9'!I12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E12" s="75">
+        <v>12.944776119402986</v>
+      </c>
+      <c r="E12" s="83">
         <f>SKX!K12</f>
         <v>1.5806688107190898</v>
       </c>
-      <c r="F12" s="75" t="e">
+      <c r="F12" s="83">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.6884386587398077</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="75">
+      <c r="C13" s="83">
         <f>'V100'!P13</f>
         <v>9.6658097686375335</v>
       </c>
-      <c r="D13" s="75" t="e">
+      <c r="D13" s="83">
         <f>'Gen9'!I13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" s="75" t="e">
+        <v>24.306638655462187</v>
+      </c>
+      <c r="E13" s="83" t="e">
         <f>SKX!K13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F13" s="75" t="e">
+      <c r="F13" s="83" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -4252,126 +4341,126 @@
       <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="75" t="e">
+      <c r="F15" s="83" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="75">
+      <c r="C16" s="83">
         <f t="shared" ref="C16:E17" si="1">C4</f>
         <v>49.802056555269928</v>
       </c>
-      <c r="D16" s="75" t="e">
+      <c r="D16" s="83">
+        <f t="shared" si="1"/>
+        <v>48.713924358142258</v>
+      </c>
+      <c r="E16" s="83">
+        <f t="shared" si="1"/>
+        <v>35.89118902039673</v>
+      </c>
+      <c r="F16" s="83">
+        <f>3/(1/C16+1/D16+1/E16)</f>
+        <v>43.815132568145579</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="83">
+        <f t="shared" si="1"/>
+        <v>91.669665809768645</v>
+      </c>
+      <c r="D17" s="83">
+        <f t="shared" si="1"/>
+        <v>30.516417910447764</v>
+      </c>
+      <c r="E17" s="83" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E16" s="75">
-        <f t="shared" si="1"/>
-        <v>35.89118902039673</v>
-      </c>
-      <c r="F16" s="75" t="e">
-        <f>3/(1/C16+1/D16+1/E16)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="75">
-        <f t="shared" si="1"/>
-        <v>91.669665809768645</v>
-      </c>
-      <c r="D17" s="75" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="75" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="75" t="e">
+      <c r="F17" s="83">
         <f>2/(1/C17+1/D17)</f>
-        <v>#DIV/0!</v>
+        <v>45.7896635424961</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="75">
+      <c r="C18" s="83">
         <f>C8</f>
         <v>92.9043701799486</v>
       </c>
-      <c r="D18" s="75" t="e">
+      <c r="D18" s="83">
         <f t="shared" ref="D18" si="2">D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="75">
+        <v>20.789552238805971</v>
+      </c>
+      <c r="E18" s="83">
         <f>E8</f>
         <v>9.9794638656180137</v>
       </c>
-      <c r="F18" s="75" t="e">
+      <c r="F18" s="83">
         <f t="shared" ref="F18:F20" si="3">3/(1/C18+1/D18+1/E18)</f>
-        <v>#DIV/0!</v>
+        <v>18.859547530583541</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="75">
+      <c r="C19" s="83">
         <f t="shared" ref="C19:E20" si="4">C10</f>
         <v>35.500000000000007</v>
       </c>
-      <c r="D19" s="75" t="e">
+      <c r="D19" s="83">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="75">
+        <v>40.320895522388071</v>
+      </c>
+      <c r="E19" s="83">
         <f t="shared" si="4"/>
         <v>78.157447959792606</v>
       </c>
-      <c r="F19" s="75" t="e">
+      <c r="F19" s="83">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>45.617152300957841</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="75">
+      <c r="C20" s="83">
         <f t="shared" si="4"/>
         <v>72.407455012853447</v>
       </c>
-      <c r="D20" s="75" t="e">
+      <c r="D20" s="83">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="75">
+        <v>96.031343283582103</v>
+      </c>
+      <c r="E20" s="83">
         <f t="shared" si="4"/>
         <v>16.478459679711456</v>
       </c>
-      <c r="F20" s="75" t="e">
+      <c r="F20" s="83">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>35.33182581495447</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
@@ -4391,27 +4480,27 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="8"/>
-      <c r="C24" s="86"/>
+      <c r="C24" s="94"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
-      <c r="C25" s="86"/>
+      <c r="C25" s="94"/>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
-      <c r="C26" s="86"/>
+      <c r="C26" s="94"/>
       <c r="D26" s="8"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
-      <c r="C27" s="86"/>
+      <c r="C27" s="94"/>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
-      <c r="C28" s="86"/>
+      <c r="C28" s="94"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -4438,193 +4527,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="83" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="76">
+      <c r="B2" s="84">
         <f>'V100'!I14</f>
         <v>631.66999999999996</v>
       </c>
-      <c r="C2" s="76">
+      <c r="C2" s="84">
         <f>'Gen9'!E16</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="76">
+        <v>626.74942399999998</v>
+      </c>
+      <c r="D2" s="84">
         <f>SKX!E15</f>
         <v>658.88131200500004</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="84">
         <f>'V100'!I15</f>
         <v>18547.65264</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="84">
         <f>'Gen9'!E17</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="76">
+        <v>18493.694954999999</v>
+      </c>
+      <c r="D3" s="84">
         <f>SKX!E16</f>
         <v>18547.652640003998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="84">
         <f>'V100'!I16</f>
         <v>7.5497584000000006E-2</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="84">
         <f>'Gen9'!E18</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="76">
+        <v>6.900996999999999E-2</v>
+      </c>
+      <c r="D5" s="84">
         <f>SKX!E17</f>
         <v>7.5497584000000006E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="84">
         <f>'V100'!I17</f>
         <v>1.6252928E-2</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="84">
         <f>'Gen9'!E19</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="76">
+        <v>1.924377E-2</v>
+      </c>
+      <c r="D6" s="84">
         <f>SKX!E18</f>
         <v>2.4641535999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="84">
         <f>'V100'!I18</f>
         <v>0.50390040000000003</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="84">
         <f>'Gen9'!E20</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="76">
+        <v>21.844860000000001</v>
+      </c>
+      <c r="D7" s="84">
         <f>SKX!E19</f>
         <v>10.035029</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="84">
         <f>'V100'!I19</f>
         <v>81.401020415999994</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="84">
         <f>'Gen9'!E21</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="76">
+        <v>174.55414752000001</v>
+      </c>
+      <c r="D8" s="84">
         <f>SKX!E20</f>
         <v>81.470365841000003</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="84">
         <f>'V100'!I20</f>
         <v>20.342517730000001</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="84">
         <f>'Gen9'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="76">
+        <v>239.31979999999996</v>
+      </c>
+      <c r="D9" s="84">
         <f>SKX!E21</f>
         <v>1.6280999999999999E-5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="76">
+      <c r="B10" s="84">
         <f>'V100'!I21</f>
         <v>6297.7459424879999</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="84">
         <f>'Gen9'!E23</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="76">
+        <v>4809.9228000000003</v>
+      </c>
+      <c r="D10" s="84">
         <f>SKX!E22</f>
         <v>3148.873729506</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="76">
+      <c r="B11" s="84">
         <f>'V100'!I22</f>
         <v>3.5651584000000001</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="84">
         <f>'Gen9'!E24</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="76">
+        <v>3.7748735999999998</v>
+      </c>
+      <c r="D11" s="84">
         <f>SKX!E23</f>
         <v>3.5651584000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="76">
+      <c r="B12" s="84">
         <f>'V100'!I23</f>
         <v>1.8682907200000001</v>
       </c>
-      <c r="C12" s="76">
+      <c r="C12" s="84">
         <f>'Gen9'!E25</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="76">
+        <v>182.66460800000002</v>
+      </c>
+      <c r="D12" s="84">
         <f>SKX!E24</f>
         <v>220.849212771</v>
       </c>
@@ -4688,202 +4777,202 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="83" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="83">
         <f>'V100'!K3</f>
         <v>5.0184476632959818</v>
       </c>
-      <c r="E4" s="75" t="e">
+      <c r="E4" s="83">
         <f>'Gen9'!D3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" s="75">
+        <v>5.9156735184780231</v>
+      </c>
+      <c r="F4" s="83">
         <f>SKX!G3</f>
         <v>6.2189554230017672</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="83">
         <f>'V100'!K4</f>
         <v>4.4738178918438845</v>
       </c>
-      <c r="E5" s="75" t="e">
+      <c r="E5" s="83">
         <f>'Gen9'!D4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="75">
+        <v>2.870172237860491</v>
+      </c>
+      <c r="F5" s="83">
         <f>SKX!G4</f>
         <v>3.4287012519750459</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="75">
+      <c r="D6" s="83">
         <f>'V100'!K5</f>
         <v>0.54960285195032399</v>
       </c>
-      <c r="E6" s="75" t="e">
+      <c r="E6" s="83">
         <f>'Gen9'!D5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="75">
+        <v>0.48425119827839191</v>
+      </c>
+      <c r="F6" s="83">
         <f>SKX!G5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="75">
+      <c r="D7" s="83">
         <f>'V100'!K6</f>
         <v>0.22560685799913865</v>
       </c>
-      <c r="E7" s="75" t="e">
+      <c r="E7" s="83">
         <f>'Gen9'!D6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="75">
+        <v>0.26287058823529413</v>
+      </c>
+      <c r="F7" s="83">
         <f>SKX!G6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="75">
+      <c r="D8" s="83">
         <f>'V100'!K7</f>
         <v>1.0893389656695045</v>
       </c>
-      <c r="E8" s="75" t="e">
+      <c r="E8" s="83">
         <f>'Gen9'!D7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="75">
+        <v>2.0319174466042718</v>
+      </c>
+      <c r="F8" s="83">
         <f>SKX!G7</f>
         <v>1.6794649840847096</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="83">
         <f>'V100'!K8</f>
         <v>0.73166262605702104</v>
       </c>
-      <c r="E9" s="75" t="e">
+      <c r="E9" s="83">
         <f>'Gen9'!D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="75">
+        <v>1.481226218680451</v>
+      </c>
+      <c r="F9" s="83">
         <f>SKX!G8</f>
         <v>1.9374609905265496</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="83">
         <f>'V100'!K9</f>
         <v>98.03108823446361</v>
       </c>
-      <c r="E10" s="75" t="e">
+      <c r="E10" s="83">
         <f>'Gen9'!D9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="75">
+        <v>38.831894362620616</v>
+      </c>
+      <c r="F10" s="83">
         <f>SKX!G9</f>
         <v>6.2251728742092618E-6</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="75">
+      <c r="D11" s="83">
         <f>'V100'!K10</f>
         <v>2.9207407325538304</v>
       </c>
-      <c r="E11" s="75" t="e">
+      <c r="E11" s="83">
         <f>'Gen9'!D10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="75">
+        <v>0.80103646122524519</v>
+      </c>
+      <c r="F11" s="83">
         <f>SKX!G10</f>
         <v>0.27594973429956932</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="75">
+      <c r="D12" s="83">
         <f>'V100'!K11</f>
         <v>1.5460037615666171</v>
       </c>
-      <c r="E12" s="75" t="e">
+      <c r="E12" s="83">
         <f>'Gen9'!D11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="75">
+        <v>1.5364740320605912</v>
+      </c>
+      <c r="F12" s="83">
         <f>SKX!G11</f>
         <v>3.6214266791702761</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="75">
+      <c r="D13" s="83">
         <f>'V100'!K12</f>
         <v>0.10438777936706597</v>
       </c>
-      <c r="E13" s="75" t="e">
+      <c r="E13" s="83">
         <f>'Gen9'!D12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="75" t="e">
+        <v>5.9227487605211575</v>
+      </c>
+      <c r="F13" s="83" t="e">
         <f>SKX!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="75">
+      <c r="D14" s="83">
         <f>'V100'!K13</f>
         <v>0.20827406920480956</v>
       </c>
-      <c r="E14" s="75" t="e">
+      <c r="E14" s="83">
         <f>'Gen9'!D13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="75">
+        <v>33.350513086590574</v>
+      </c>
+      <c r="F14" s="83">
         <f>SKX!G12</f>
         <v>30.709867170058097</v>
       </c>
@@ -4892,103 +4981,103 @@
       <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="75" t="str">
+      <c r="D17" s="83" t="str">
         <f>D3</f>
         <v>V100</v>
       </c>
-      <c r="E17" s="75" t="str">
+      <c r="E17" s="83" t="str">
         <f t="shared" ref="E17:F17" si="0">E3</f>
         <v>Gen9</v>
       </c>
-      <c r="F17" s="75" t="str">
+      <c r="F17" s="83" t="str">
         <f t="shared" si="0"/>
         <v>SKX</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="75">
+      <c r="D18" s="83">
         <f>D5</f>
         <v>4.4738178918438845</v>
       </c>
-      <c r="E18" s="75" t="e">
+      <c r="E18" s="83">
         <f t="shared" ref="E18:F18" si="1">E5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="75">
+        <v>2.870172237860491</v>
+      </c>
+      <c r="F18" s="83">
         <f t="shared" si="1"/>
         <v>3.4287012519750459</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="75">
+      <c r="D19" s="83">
         <f>D6</f>
         <v>0.54960285195032399</v>
       </c>
-      <c r="E19" s="75" t="e">
+      <c r="E19" s="83">
         <f t="shared" ref="E19:F19" si="2">E6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="75">
+        <v>0.48425119827839191</v>
+      </c>
+      <c r="F19" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="75">
+      <c r="D20" s="83">
         <f>D9</f>
         <v>0.73166262605702104</v>
       </c>
-      <c r="E20" s="75" t="e">
+      <c r="E20" s="83">
         <f t="shared" ref="E20:F20" si="3">E9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="75">
+        <v>1.481226218680451</v>
+      </c>
+      <c r="F20" s="83">
         <f t="shared" si="3"/>
         <v>1.9374609905265496</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="75">
+      <c r="D21" s="83">
         <f>D11</f>
         <v>2.9207407325538304</v>
       </c>
-      <c r="E21" s="75" t="e">
+      <c r="E21" s="83">
         <f>E11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" s="75">
+        <v>0.80103646122524519</v>
+      </c>
+      <c r="F21" s="83">
         <f t="shared" ref="F21" si="4">F11</f>
         <v>0.27594973429956932</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="75">
+      <c r="D22" s="83">
         <f>D12</f>
         <v>1.5460037615666171</v>
       </c>
-      <c r="E22" s="75" t="e">
+      <c r="E22" s="83">
         <f t="shared" ref="E22:F22" si="5">E12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" s="75">
+        <v>1.5364740320605912</v>
+      </c>
+      <c r="F22" s="83">
         <f t="shared" si="5"/>
         <v>3.6214266791702761</v>
       </c>
@@ -5012,100 +5101,100 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="83" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="84">
         <f>SKX!F4</f>
         <v>76.807144503649013</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="84">
         <f>'Gen9'!C4</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="76">
+        <v>32.638329319955311</v>
+      </c>
+      <c r="D5" s="84">
         <f>'V100'!J4</f>
         <v>387.46000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="84">
         <f>SKX!F5</f>
         <v>0</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="84">
         <f>'Gen9'!C5</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="76">
+        <v>20.445999999999998</v>
+      </c>
+      <c r="D6" s="84">
         <f>'V100'!J5</f>
         <v>713.19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="84">
         <f>SKX!F8</f>
         <v>21.356052672422553</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="84">
         <f>'Gen9'!C8</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="76">
+        <v>13.929</v>
+      </c>
+      <c r="D7" s="84">
         <f>'V100'!J8</f>
         <v>722.79600000000005</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="84">
         <f>SKX!F10</f>
         <v>167.25693863395617</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="84">
         <f>'Gen9'!C10</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="76">
+        <v>27.015000000000001</v>
+      </c>
+      <c r="D8" s="84">
         <f>'V100'!J10</f>
         <v>276.19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="84">
         <f>SKX!F11</f>
         <v>35.263903714582511</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="84">
         <f>'Gen9'!C11</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="76">
+        <v>64.341000000000008</v>
+      </c>
+      <c r="D9" s="84">
         <f>'V100'!J11</f>
         <v>563.32999999999993</v>
       </c>

</xml_diff>